<commit_message>
solving matchin issues. and finalising main database
</commit_message>
<xml_diff>
--- a/clean_databases/intermediate/species_import_group.xlsx
+++ b/clean_databases/intermediate/species_import_group.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11320" yWindow="460" windowWidth="14620" windowHeight="15080" tabRatio="500"/>
+    <workbookView xWindow="10980" yWindow="460" windowWidth="14620" windowHeight="15080" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="129">
   <si>
     <t>name_sp</t>
   </si>
@@ -120,9 +120,6 @@
   </si>
   <si>
     <t>caracoles excepto los de mar</t>
-  </si>
-  <si>
-    <t>camaron_no_mar</t>
   </si>
   <si>
     <t>caviar</t>
@@ -401,6 +398,24 @@
   </si>
   <si>
     <t>trucha</t>
+  </si>
+  <si>
+    <t>caracol_no_mar</t>
+  </si>
+  <si>
+    <t>anguila</t>
+  </si>
+  <si>
+    <t>anguilas</t>
+  </si>
+  <si>
+    <t>los demas camarones, langostinos y natantia</t>
+  </si>
+  <si>
+    <t>loco</t>
+  </si>
+  <si>
+    <t>Concholepas concholepas</t>
   </si>
 </sst>
 </file>
@@ -719,10 +734,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C65"/>
+  <dimension ref="A1:C68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C66" sqref="C66"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -806,640 +821,673 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>125</v>
       </c>
       <c r="B8" t="s">
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
         <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
         <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
         <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B15" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B16" t="s">
         <v>4</v>
       </c>
       <c r="C16" t="s">
-        <v>32</v>
+        <v>123</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B17" t="s">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="C17" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B18" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C18" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B19" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="C19" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B20" t="s">
         <v>4</v>
       </c>
       <c r="C20" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
+        <v>4</v>
       </c>
       <c r="C21" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B22" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C22" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B23" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" t="s">
         <v>45</v>
       </c>
-      <c r="B24" t="s">
-        <v>47</v>
-      </c>
       <c r="C24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B25" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B26" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B27" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B28" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C28" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>45</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>52</v>
+        <v>44</v>
+      </c>
+      <c r="B29" t="s">
+        <v>50</v>
       </c>
       <c r="C29" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>53</v>
-      </c>
-      <c r="B30" t="s">
-        <v>54</v>
+        <v>44</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>51</v>
       </c>
       <c r="C30" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B31" t="s">
-        <v>4</v>
+        <v>53</v>
       </c>
       <c r="C31" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B32" t="s">
-        <v>58</v>
+        <v>4</v>
       </c>
       <c r="C32" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>56</v>
+      </c>
+      <c r="B33" t="s">
+        <v>57</v>
+      </c>
+      <c r="C33" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>59</v>
+      </c>
+      <c r="B34" t="s">
+        <v>4</v>
+      </c>
+      <c r="C34" t="s">
         <v>60</v>
       </c>
-      <c r="B33" t="s">
-        <v>4</v>
-      </c>
-      <c r="C33" t="s">
+    </row>
+    <row r="35" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" ht="48" x14ac:dyDescent="0.2">
-      <c r="A34" s="2" t="s">
+      <c r="B35" t="s">
+        <v>4</v>
+      </c>
+      <c r="C35" t="s">
         <v>62</v>
-      </c>
-      <c r="B34" t="s">
-        <v>4</v>
-      </c>
-      <c r="C34" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="64" x14ac:dyDescent="0.2">
-      <c r="A35" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B35" t="s">
-        <v>65</v>
-      </c>
-      <c r="C35" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B36" t="s">
         <v>64</v>
       </c>
-      <c r="B36" t="s">
-        <v>67</v>
-      </c>
       <c r="C36" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B37" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C37" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>69</v>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="64" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
+        <v>63</v>
       </c>
       <c r="B38" t="s">
-        <v>4</v>
+        <v>67</v>
       </c>
       <c r="C38" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B39" t="s">
         <v>4</v>
       </c>
       <c r="C39" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>73</v>
+      <c r="A40" s="2" t="s">
+        <v>127</v>
       </c>
       <c r="B40" t="s">
-        <v>4</v>
+        <v>128</v>
       </c>
       <c r="C40" t="s">
-        <v>74</v>
+        <v>127</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B41" t="s">
         <v>4</v>
       </c>
       <c r="C41" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B42" t="s">
         <v>4</v>
       </c>
       <c r="C42" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>79</v>
+        <v>126</v>
       </c>
       <c r="B43" t="s">
         <v>4</v>
       </c>
       <c r="C43" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B44" t="s">
         <v>4</v>
       </c>
       <c r="C44" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="B45" t="s">
         <v>4</v>
       </c>
       <c r="C45" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B46" t="s">
         <v>4</v>
       </c>
       <c r="C46" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="B47" t="s">
         <v>4</v>
       </c>
       <c r="C47" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B48" t="s">
         <v>4</v>
       </c>
       <c r="C48" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="B49" t="s">
         <v>4</v>
       </c>
       <c r="C49" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="B50" t="s">
-        <v>94</v>
+        <v>4</v>
       </c>
       <c r="C50" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="B51" t="s">
         <v>4</v>
       </c>
       <c r="C51" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="B52" t="s">
         <v>4</v>
       </c>
       <c r="C52" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B53" t="s">
-        <v>4</v>
+        <v>93</v>
       </c>
       <c r="C53" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B54" t="s">
-        <v>102</v>
+        <v>4</v>
       </c>
       <c r="C54" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="B55" t="s">
-        <v>105</v>
+        <v>4</v>
       </c>
       <c r="C55" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>107</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>108</v>
+        <v>99</v>
+      </c>
+      <c r="B56" t="s">
+        <v>4</v>
       </c>
       <c r="C56" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>107</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>110</v>
+        <v>100</v>
+      </c>
+      <c r="B57" t="s">
+        <v>101</v>
       </c>
       <c r="C57" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="B58" t="s">
-        <v>4</v>
+        <v>104</v>
       </c>
       <c r="C58" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>113</v>
-      </c>
-      <c r="B59" t="s">
-        <v>4</v>
+        <v>106</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>107</v>
       </c>
       <c r="C59" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>115</v>
-      </c>
-      <c r="B60" t="s">
-        <v>4</v>
+        <v>106</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>109</v>
       </c>
       <c r="C60" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="B61" t="s">
         <v>4</v>
       </c>
       <c r="C61" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B62" t="s">
         <v>4</v>
       </c>
       <c r="C62" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B63" t="s">
         <v>4</v>
       </c>
       <c r="C63" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="B64" t="s">
         <v>4</v>
       </c>
       <c r="C64" t="s">
-        <v>32</v>
+        <v>116</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B65" t="s">
         <v>4</v>
       </c>
       <c r="C65" t="s">
-        <v>123</v>
+        <v>118</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>119</v>
+      </c>
+      <c r="B66" t="s">
+        <v>4</v>
+      </c>
+      <c r="C66" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>121</v>
+      </c>
+      <c r="B67" t="s">
+        <v>4</v>
+      </c>
+      <c r="C67" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>122</v>
+      </c>
+      <c r="B68" t="s">
+        <v>4</v>
+      </c>
+      <c r="C68" t="s">
+        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>